<commit_message>
fix and added new dbs
-fixed yAxis title
-added new dbs.
</commit_message>
<xml_diff>
--- a/תעדוף משימות מתפש.xlsx
+++ b/תעדוף משימות מתפש.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ishai\Desktop\matpash-04-11-20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ishai\Documents\GitHub\matpash-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CDF3C9-9ECE-417B-8444-CDA28FB35FC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03541E8-C056-4B66-86FA-EDE803F642B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="868" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="כללי" sheetId="12" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
   <si>
     <t>משימות:</t>
   </si>
@@ -378,9 +378,6 @@
   </si>
   <si>
     <t>לדאוג שעבור משתמש יוצג התפריט הנכון לפי הרשאה (בגרף)</t>
-  </si>
-  <si>
-    <t>עד 30/11</t>
   </si>
   <si>
     <t>30/11</t>
@@ -769,7 +766,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1071,15 +1068,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="29.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.8984375" customWidth="1"/>
-    <col min="2" max="2" width="20.3984375" customWidth="1"/>
+    <col min="1" max="1" width="33.875" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="34.19921875" customWidth="1"/>
+    <col min="4" max="4" width="34.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1084,7 @@
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1101,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>49</v>
       </c>
@@ -1113,7 +1110,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>54</v>
       </c>
@@ -1122,10 +1119,10 @@
         <v>29</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>55</v>
       </c>
@@ -1135,7 +1132,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>70</v>
       </c>
@@ -1147,7 +1144,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
         <v>72</v>
       </c>
@@ -1157,7 +1154,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>73</v>
       </c>
@@ -1182,12 +1179,12 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1192,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1209,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>30</v>
       </c>
@@ -1221,7 +1218,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>64</v>
       </c>
@@ -1233,7 +1230,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>65</v>
       </c>
@@ -1245,7 +1242,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>66</v>
       </c>
@@ -1257,17 +1254,17 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="36"/>
       <c r="B9" s="24"/>
       <c r="C9" s="37"/>
     </row>
-    <row r="10" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>79</v>
       </c>
@@ -1278,10 +1275,10 @@
         <v>44165</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="39"/>
       <c r="B11" s="24"/>
       <c r="C11" s="41"/>
@@ -1304,15 +1301,15 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.8984375" customWidth="1"/>
+    <col min="1" max="1" width="39.875" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" customWidth="1"/>
-    <col min="4" max="4" width="42.3984375" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="42.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -1320,7 +1317,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1334,7 +1331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -1346,7 +1343,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1358,7 +1355,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
@@ -1370,7 +1367,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>46</v>
       </c>
@@ -1384,7 +1381,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>95</v>
       </c>
@@ -1398,7 +1395,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>97</v>
       </c>
@@ -1410,7 +1407,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>96</v>
       </c>
@@ -1422,7 +1419,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>53</v>
       </c>
@@ -1434,7 +1431,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>63</v>
       </c>
@@ -1446,19 +1443,19 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
       <c r="C12" s="26"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="26"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
     </row>
   </sheetData>
@@ -1473,19 +1470,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986CB6E6-5CE8-42A8-B6BC-447AA4624483}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="37.19921875" customWidth="1"/>
+    <col min="1" max="1" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="37.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -1493,7 +1490,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1507,7 +1504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -1519,7 +1516,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1531,7 +1528,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
@@ -1543,7 +1540,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
@@ -1555,7 +1552,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -1567,7 +1564,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>40</v>
       </c>
@@ -1579,7 +1576,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>41</v>
       </c>
@@ -1591,7 +1588,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>44</v>
       </c>
@@ -1603,7 +1600,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>7</v>
       </c>
@@ -1615,7 +1612,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>74</v>
       </c>
@@ -1627,7 +1624,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>45</v>
       </c>
@@ -1641,7 +1638,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>56</v>
       </c>
@@ -1653,19 +1650,19 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>104</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>105</v>
+      <c r="C15" s="17" t="s">
+        <v>4</v>
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>47</v>
       </c>
@@ -1677,13 +1674,13 @@
       </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
       <c r="B17" s="28"/>
     </row>
-    <row r="18" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>88</v>
       </c>
@@ -1693,10 +1690,10 @@
       </c>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="28"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="29"/>
     </row>
   </sheetData>
@@ -1715,16 +1712,16 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="35.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.59765625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="44.625" style="15" customWidth="1"/>
     <col min="2" max="2" width="12" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.8984375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="46.69921875" style="15" customWidth="1"/>
-    <col min="5" max="16384" width="35.8984375" style="15"/>
+    <col min="3" max="3" width="13.875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="46.75" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="35.875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -1732,7 +1729,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1746,7 +1743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -1758,7 +1755,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1770,7 +1767,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
@@ -1782,7 +1779,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>28</v>
       </c>
@@ -1791,10 +1788,10 @@
         <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>39</v>
       </c>
@@ -1806,7 +1803,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
@@ -1818,7 +1815,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>42</v>
       </c>
@@ -1830,7 +1827,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>43</v>
       </c>
@@ -1842,7 +1839,7 @@
       </c>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>57</v>
       </c>
@@ -1854,7 +1851,7 @@
       </c>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>51</v>
       </c>
@@ -1866,7 +1863,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>50</v>
       </c>
@@ -1878,7 +1875,7 @@
       </c>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>71</v>
       </c>
@@ -1890,7 +1887,7 @@
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>38</v>
       </c>
@@ -1904,12 +1901,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>86</v>
       </c>
@@ -1923,7 +1920,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>87</v>
       </c>
@@ -1937,12 +1934,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>91</v>
       </c>
@@ -1972,15 +1969,15 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.8984375" customWidth="1"/>
-    <col min="3" max="3" width="14.8984375" customWidth="1"/>
-    <col min="4" max="4" width="16.69921875" customWidth="1"/>
+    <col min="1" max="1" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -1988,7 +1985,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2002,7 +1999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -2014,7 +2011,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
@@ -2026,7 +2023,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
@@ -2038,7 +2035,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>58</v>
       </c>
@@ -2050,13 +2047,13 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="25"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>78</v>
       </c>
@@ -2064,7 +2061,7 @@
       <c r="C8" s="24"/>
       <c r="D8" s="25"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>84</v>
       </c>
@@ -2085,15 +2082,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.59765625" customWidth="1"/>
-    <col min="2" max="2" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.09765625" customWidth="1"/>
+    <col min="1" max="1" width="40.625" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -2101,7 +2098,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2115,7 +2112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -2127,7 +2124,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -2139,7 +2136,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -2151,7 +2148,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
@@ -2163,7 +2160,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -2175,7 +2172,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>83</v>
       </c>
@@ -2189,7 +2186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -2207,19 +2204,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4AC204-14A0-4D78-88CF-487A5065FC8A}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -2227,7 +2224,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2241,7 +2238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -2253,7 +2250,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
@@ -2265,7 +2262,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
@@ -2277,7 +2274,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2285,7 +2282,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
@@ -2297,7 +2294,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>59</v>
       </c>
@@ -2309,7 +2306,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>52</v>
       </c>
@@ -2321,7 +2318,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -2329,7 +2326,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
@@ -2341,7 +2338,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2353,7 +2350,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -2365,7 +2362,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2373,7 +2370,7 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
@@ -2385,7 +2382,7 @@
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>32</v>
       </c>
@@ -2399,7 +2396,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>33</v>
       </c>
@@ -2411,7 +2408,7 @@
       </c>
       <c r="D17" s="45"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>77</v>
       </c>
@@ -2421,26 +2418,26 @@
       </c>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>84</v>
       </c>
@@ -2463,12 +2460,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -2476,7 +2473,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2490,7 +2487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -2502,7 +2499,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
@@ -2514,7 +2511,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
@@ -2526,7 +2523,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>60</v>
       </c>
@@ -2538,7 +2535,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>61</v>
       </c>
@@ -2550,12 +2547,12 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>81</v>
       </c>
@@ -2576,15 +2573,15 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.59765625" customWidth="1"/>
+    <col min="1" max="1" width="57.625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="23.3984375" customWidth="1"/>
+    <col min="4" max="4" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -2592,7 +2589,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2606,7 +2603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -2618,7 +2615,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -2630,7 +2627,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -2642,7 +2639,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
@@ -2654,7 +2651,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
flip and yAxis Title
added flip option checkbox for reverse timeline for xAxis
added yAxis title

changed dbs
</commit_message>
<xml_diff>
--- a/תעדוף משימות מתפש.xlsx
+++ b/תעדוף משימות מתפש.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ishai\Documents\GitHub\matpash-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03541E8-C056-4B66-86FA-EDE803F642B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D616A4C-21FC-4633-B76A-1A3FF144A648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="114">
   <si>
     <t>משימות:</t>
   </si>
@@ -200,9 +200,6 @@
     <t>מחיקת גרף מדשבורד</t>
   </si>
   <si>
-    <t>אופציה לבחירת דשבורד שיופיע בכניסה למסך</t>
-  </si>
-  <si>
     <t>העלאת אקסלים חדשים/מעודכנים</t>
   </si>
   <si>
@@ -399,6 +396,15 @@
   </si>
   <si>
     <t>Factory method for different graphs/service</t>
+  </si>
+  <si>
+    <t>עד ה30.11</t>
+  </si>
+  <si>
+    <t>אופציה לבחירת דשבורד שיופיע בכניסה למסך - הוספת כפתור ברירת מחדל</t>
+  </si>
+  <si>
+    <t>שינוי מיקום הכותרת והכפתורים. בחירה בצד ומחיקה ושמירה בצד</t>
   </si>
 </sst>
 </file>
@@ -1100,31 +1106,31 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="26" t="s">
@@ -1134,19 +1140,19 @@
     </row>
     <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="17" t="s">
@@ -1156,14 +1162,14 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1220,7 +1226,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -1232,7 +1238,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -1244,7 +1250,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
@@ -1256,7 +1262,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1266,16 +1272,16 @@
     </row>
     <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>79</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="C10" s="42">
         <v>44165</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1369,7 +1375,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>13</v>
@@ -1378,12 +1384,12 @@
         <v>29</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
@@ -1392,12 +1398,12 @@
         <v>29</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -1409,7 +1415,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -1421,7 +1427,7 @@
     </row>
     <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
@@ -1433,7 +1439,7 @@
     </row>
     <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>13</v>
@@ -1468,15 +1474,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986CB6E6-5CE8-42A8-B6BC-447AA4624483}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55" customWidth="1"/>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="37.25" customWidth="1"/>
@@ -1509,7 +1515,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>4</v>
@@ -1533,7 +1539,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>4</v>
@@ -1545,7 +1551,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>4</v>
@@ -1557,7 +1563,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>4</v>
@@ -1569,7 +1575,7 @@
         <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>4</v>
@@ -1581,7 +1587,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>4</v>
@@ -1593,7 +1599,7 @@
         <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>4</v>
@@ -1605,7 +1611,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>4</v>
@@ -1614,48 +1620,48 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C12" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>45</v>
+      <c r="A13" s="31" t="s">
+        <v>113</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>98</v>
-      </c>
+      <c r="C13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>4</v>
@@ -1664,37 +1670,49 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="28"/>
-    </row>
-    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="26" t="s">
+      <c r="C17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="28"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="29"/>
+      <c r="B20" s="28"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1708,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2305990A-13DC-4229-BE5A-7F8711EF7D31}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView rightToLeft="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1748,7 +1766,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>4</v>
@@ -1788,7 +1806,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1841,7 +1859,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>20</v>
@@ -1853,19 +1871,19 @@
     </row>
     <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>20</v>
@@ -1877,7 +1895,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>20</v>
@@ -1898,31 +1916,31 @@
         <v>29</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>20</v>
@@ -1931,17 +1949,17 @@
         <v>29</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>20</v>
@@ -1950,7 +1968,7 @@
         <v>29</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2037,7 +2055,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>13</v>
@@ -2055,7 +2073,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
@@ -2063,7 +2081,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2174,16 +2192,16 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2296,7 +2314,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -2308,7 +2326,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -2393,7 +2411,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2410,7 +2428,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="17" t="s">
@@ -2420,26 +2438,26 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2525,7 +2543,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>13</v>
@@ -2537,7 +2555,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
@@ -2549,12 +2567,12 @@
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2653,7 +2671,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>20</v>

</xml_diff>